<commit_message>
simple regression in notebook
</commit_message>
<xml_diff>
--- a/skostr_hoyde.xlsx
+++ b/skostr_hoyde.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theabj/Box Sync/Undervisning/statistikk_ingeniører/ISTX100YH23/forprosjekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erik/PycharmProjects/PNS/istg1003forprosjekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6D9FC5-E7A0-B74B-A09F-893EB43A5DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4235D3B6-6D32-1D47-A144-9B135AADCF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5500" yWindow="2060" windowWidth="22060" windowHeight="13780" xr2:uid="{17AD7C0B-BD46-864B-A286-7DB13EBD5FC9}"/>
   </bookViews>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A645C9-12C5-5C40-AEE3-FEEA757065DC}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,6 +449,54 @@
         <v>161</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>